<commit_message>
updated model training scripts
</commit_message>
<xml_diff>
--- a/roadvisionSheet.xlsx
+++ b/roadvisionSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taiwoadelakin/Documents/Doc/Projects/roadvision/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA42B71B-5C3C-DD4F-9F83-BC13572840C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F89341A2-C8C0-3547-863F-2A9213017928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1060" yWindow="500" windowWidth="27740" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="5">
   <si>
     <t>vision</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t>SpeedBump</t>
+  </si>
+  <si>
+    <t>speed-bumps-and-potholes</t>
   </si>
 </sst>
 </file>
@@ -878,7 +881,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -962,10 +965,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{699E91B4-F905-3C4A-8B08-123281C029EC}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -980,16 +983,21 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>